<commit_message>
TC_AddCustomerTEST_003.java test case 3 added
</commit_message>
<xml_diff>
--- a/src/test/java/com/netbanking/testData/LoginData.xlsx
+++ b/src/test/java/com/netbanking/testData/LoginData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -36,6 +36,18 @@
   </si>
   <si>
     <t>aguzApy</t>
+  </si>
+  <si>
+    <t>mngr464119</t>
+  </si>
+  <si>
+    <t>mngr464120</t>
+  </si>
+  <si>
+    <t>mngr464121</t>
+  </si>
+  <si>
+    <t>mngr464122</t>
   </si>
 </sst>
 </file>
@@ -364,9 +376,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -392,7 +402,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
@@ -400,7 +410,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
         <v>3</v>
@@ -408,7 +418,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -416,7 +426,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
         <v>3</v>

</xml_diff>